<commit_message>
Created health class & refactored avatar class
</commit_message>
<xml_diff>
--- a/1DAE21_Belmans_Jef_CaveCrawler/Belmans_Jef_Game.xlsx
+++ b/1DAE21_Belmans_Jef_CaveCrawler/Belmans_Jef_Game.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2019_2020\_Programming2\00_GameProject\ForStudents\Description&amp;Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36BFE45F-C8CD-4784-BA45-354287853801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62453C86-B713-4E37-B9B2-AA5827C7C158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Game rubric" sheetId="2" r:id="rId1"/>
@@ -512,7 +512,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -540,7 +540,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -729,6 +729,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m99485b88215436a82099f8287cba0b0>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100723942CCEB3A674D8F1F6472CCEFB38E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b456a193ed59fb7b1c8994f62cf0bc67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="128482ec-0431-40d5-ab26-89ea2a4f3ccd" xmlns:ns3="60eb0cf4-ae2a-4762-800a-cb593b869ecb" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns5="a2e691a9-fcfc-4d85-a390-1894fe98bd9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a253e5da7d9e3ac9660eca9ce8fbd104" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
@@ -981,35 +1002,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m99485b88215436a82099f8287cba0b0>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBBEFD80-C66F-4B0C-9ED1-734A448E3DFF}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}"/>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}"/>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBBEFD80-C66F-4B0C-9ED1-734A448E3DFF}"/>
 </file>
</xml_diff>